<commit_message>
new file:   .gitignore 	modified:   __pycache__/app.cpython-39.pyc 	modified:   __pycache__/functions.cpython-39.pyc 	modified:   app.py 	modified:   aux data/Data.xlsx 	modified:   functions.py 	modified:   instance/db.db     new file:   static/field_values.js 	new file:   static/functions.js 	modified:   static/my_override_style.css 	modified:   templates/base.html 	new file:   templates/base_words.html 	new file:   templates/words_edit.html     new file:   templates/words_history.html 	new file:   templates/words_new.html 	new file:   templates/words_stats.html 	new file:   templates/words_view.html
</commit_message>
<xml_diff>
--- a/aux data/Data.xlsx
+++ b/aux data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhsengland-my.sharepoint.com/personal/andrew_pike9_england_nhs_uk/Documents/Desktop/NHS England/Personal/Andy Site/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhsengland-my.sharepoint.com/personal/andrew_pike9_england_nhs_uk/Documents/Desktop/NHS England/Personal/Andy Site/aux data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{7ACF4993-8E2D-4DBE-AE4F-61FF9DB71A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E8FB4B7-93D0-4EAF-AE95-4995E88DBE2F}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="8_{7ACF4993-8E2D-4DBE-AE4F-61FF9DB71A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AD49560-D43F-4D57-954B-6F40F882AF60}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{7FE89C6B-0D6B-49AE-9239-99156FA3D800}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
   <si>
     <t>home</t>
   </si>
@@ -178,13 +178,100 @@
   </si>
   <si>
     <t>Blob</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Essay</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>NHS England</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Simplify Health</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Free format</t>
+  </si>
+  <si>
+    <t>Written</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>SimplifyHealth</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>WORDS</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Edited</t>
+  </si>
+  <si>
+    <t>Latest</t>
+  </si>
+  <si>
+    <t>Date Edited</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Date Note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +301,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +321,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -237,11 +342,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,6 +445,53 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,6 +507,276 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>515938</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F31F4E9-AB63-F439-393F-0B9EA9217E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9398000" y="3921125"/>
+          <a:ext cx="1976438" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>493712</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A750FC8-3EEC-4AA4-8D7F-277B390E0834}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9304337" y="4462462"/>
+          <a:ext cx="1976438" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566737</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>98424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF400E4B-C9B2-42BC-9E38-AA63B3FDB392}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9377362" y="4662487"/>
+          <a:ext cx="806451" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>103187</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5AE8F9A-64AD-8704-6B5E-5568F3B199EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10787063" y="6635750"/>
+          <a:ext cx="785812" cy="23813"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>541338</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19083966-6228-4F00-86EE-25ED02B4FCA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9636125" y="7024688"/>
+          <a:ext cx="1763713" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1140BDB1-0EE0-42B5-B05A-EB8B94FE79F6}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,16 +1201,18 @@
     <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="2" max="3" width="14.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -719,7 +1223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -730,7 +1234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -738,15 +1242,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -756,8 +1271,15 @@
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -770,8 +1292,17 @@
       <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -782,15 +1313,82 @@
       <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -800,8 +1398,11 @@
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -811,8 +1412,11 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -820,7 +1424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -828,7 +1432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -836,7 +1440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -846,24 +1450,73 @@
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -873,16 +1526,33 @@
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N21" s="8"/>
+      <c r="O21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -892,8 +1562,16 @@
       <c r="D23" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
@@ -903,23 +1581,55 @@
       <c r="D24" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N26" s="8"/>
+      <c r="O26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="N28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -929,8 +1639,17 @@
       <c r="C29" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -940,16 +1659,34 @@
       <c r="C30" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -959,8 +1696,22 @@
       <c r="C32" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -970,8 +1721,16 @@
       <c r="C33" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -981,8 +1740,20 @@
       <c r="C34" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="I34" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
@@ -993,31 +1764,88 @@
       <c r="D35" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H37" s="9"/>
+      <c r="I37" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N37" s="9"/>
+      <c r="O37" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H38" s="9"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="9"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H39" s="9"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L39" s="18"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="9"/>
+      <c r="O39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1027,14 +1855,255 @@
       <c r="C40" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="9"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H41" s="9"/>
+      <c r="I41" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" s="9"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H42" s="9"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="9"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H43" s="9"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="9"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H44" s="9"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="9"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H45" s="9"/>
+      <c r="I45" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K45" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N45" s="9"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H46" s="9"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="9"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H47" s="9"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="K47" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L47" s="18"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="9"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H48" s="9"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="9"/>
+    </row>
+    <row r="49" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H49" s="9"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="9"/>
+    </row>
+    <row r="50" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H50" s="9"/>
+      <c r="I50" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L50" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="M50" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N50" s="9"/>
+    </row>
+    <row r="51" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H51" s="9"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="9"/>
+    </row>
+    <row r="52" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H52" s="9"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="K52" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="L52" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M52" s="19"/>
+      <c r="N52" s="9"/>
+    </row>
+    <row r="53" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H53" s="9"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="9"/>
+    </row>
+    <row r="54" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H54" s="9"/>
+      <c r="I54" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M54" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N54" s="9"/>
+    </row>
+    <row r="55" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H55" s="9"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="9"/>
+    </row>
+    <row r="56" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H56" s="9"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="9"/>
+    </row>
+    <row r="57" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+    </row>
+    <row r="58" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+    </row>
+    <row r="59" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+    </row>
+    <row r="60" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A37:C37"/>
+    <mergeCell ref="I34:M34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>